<commit_message>
criei o exercicio 22
</commit_message>
<xml_diff>
--- a/agenda controle.xlsx
+++ b/agenda controle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguia\Documents\GitHub\ProjetosEstudos\module1--html5---css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F876DB-28F8-4483-8405-0FA4A72DFBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F7774A-D6DE-4A52-A07E-66E2947801EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28785" yWindow="-15435" windowWidth="13485" windowHeight="9930" xr2:uid="{FD96FF53-C3B6-47FE-BDDB-316B30E4002C}"/>
+    <workbookView xWindow="23235" yWindow="-12360" windowWidth="18690" windowHeight="9990" xr2:uid="{FD96FF53-C3B6-47FE-BDDB-316B30E4002C}"/>
   </bookViews>
   <sheets>
     <sheet name="module3" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Total</t>
   </si>
@@ -199,6 +199,18 @@
   </si>
   <si>
     <t>Capítulo 18 Aula 07 – Manutenção em sites hospedados no GitHub Pages</t>
+  </si>
+  <si>
+    <t>Capítulo 18 Aula 08 – Recursos Sociais do GitHub</t>
+  </si>
+  <si>
+    <t>Capítulo 18 Aula 09 – Clonando Repositórios GitHub</t>
+  </si>
+  <si>
+    <t>Capítulo 18 Aula 10 – GitHub em vários PCs</t>
+  </si>
+  <si>
+    <t>Capítulo 19 Aula 01- Download das imagens do capítulo</t>
   </si>
 </sst>
 </file>
@@ -561,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6477F9D2-859D-45A0-B918-D94927AC7D3F}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -571,6 +583,7 @@
     <col min="2" max="2" width="8.83984375" style="3"/>
     <col min="3" max="4" width="8.83984375" style="1"/>
     <col min="6" max="6" width="9.83984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
@@ -744,42 +757,93 @@
       <c r="C9" s="1">
         <v>0.88194444444444453</v>
       </c>
+      <c r="D9" s="1">
+        <v>0.88888888888888884</v>
+      </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>-0.88194444444444453</v>
+        <v>6.9444444444443088E-3</v>
       </c>
       <c r="F9" s="2">
         <v>44980</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="3">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.89861111111111114</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.91041666666666676</v>
+      </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.1805555555555625E-2</v>
       </c>
       <c r="F10" s="2">
         <v>44980</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="3">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.91111111111111109</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.92013888888888884</v>
+      </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.0277777777777457E-3</v>
       </c>
       <c r="F11" s="2">
         <v>44980</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="3">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.92083333333333339</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.9375</v>
+      </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.6666666666666607E-2</v>
       </c>
       <c r="F12" s="2">
         <v>44980</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="3">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.94027777777777777</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.94027777777777777</v>
+      </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -808,464 +872,105 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4"/>
-      <c r="E16" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="1">
-        <f>SUM(E6:E16)</f>
-        <v>-0.84236111111111112</v>
-      </c>
-      <c r="J16" s="1">
-        <f>G16+G27+G38+G51</f>
-        <v>-0.48958333333333393</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="E17" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="2">
-        <v>44977</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E18" s="1"/>
-      <c r="F18" s="2">
-        <v>44977</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="G18" s="1">
+        <f>SUM(E2:E18)+module2!G51</f>
+        <v>0.25416666666666643</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E19" s="1"/>
-      <c r="F19" s="2">
-        <v>44978</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E20" s="1"/>
-      <c r="F20" s="2">
-        <v>44978</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E21" s="1"/>
-      <c r="F21" s="2">
-        <v>44978</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E22" s="1"/>
-      <c r="F22" s="2">
-        <v>44978</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E23" s="1"/>
-      <c r="F23" s="2">
-        <v>44978</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E24" s="1"/>
-      <c r="F24" s="2">
-        <v>44978</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E25" s="1"/>
-      <c r="F25" s="2">
-        <v>44978</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E26" s="1"/>
-      <c r="F26" s="2">
-        <v>44978</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F27" s="2">
-        <v>44978</v>
-      </c>
-      <c r="G27" s="1">
-        <f>SUM(E19:E27)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E28" s="1"/>
-      <c r="F28" s="2">
-        <v>44979</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E29" s="1"/>
-      <c r="F29" s="2">
-        <v>44979</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E30" s="1"/>
-      <c r="F30" s="2">
-        <v>44979</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="3">
-        <v>8</v>
-      </c>
-      <c r="C31" s="1">
-        <v>0.60069444444444442</v>
-      </c>
-      <c r="D31" s="1">
-        <v>0.61111111111111105</v>
-      </c>
-      <c r="E31" s="1">
-        <f t="shared" ref="E6:E45" si="1">D31-C31</f>
-        <v>1.041666666666663E-2</v>
-      </c>
-      <c r="F31" s="2">
-        <v>44979</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="1">
-        <v>0.625</v>
-      </c>
-      <c r="D32" s="1">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="E32" s="1">
-        <f t="shared" si="1"/>
-        <v>8.333333333333337E-2</v>
-      </c>
-      <c r="F32" s="2">
-        <v>44979</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="3">
-        <v>10</v>
-      </c>
-      <c r="C33" s="1">
-        <v>0.81944444444444453</v>
-      </c>
-      <c r="D33" s="1">
-        <v>0.82361111111111107</v>
-      </c>
-      <c r="E33" s="1">
-        <f t="shared" si="1"/>
-        <v>4.1666666666665408E-3</v>
-      </c>
-      <c r="F33" s="2">
-        <v>44979</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="3">
-        <v>9</v>
-      </c>
-      <c r="C34" s="1">
-        <v>0.83888888888888891</v>
-      </c>
-      <c r="D34" s="1">
-        <v>0.84375</v>
-      </c>
-      <c r="E34" s="1">
-        <f t="shared" si="1"/>
-        <v>4.8611111111110938E-3</v>
-      </c>
-      <c r="F34" s="2">
-        <v>44979</v>
-      </c>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="3">
-        <v>15</v>
-      </c>
-      <c r="C35" s="1">
-        <v>0.84444444444444444</v>
-      </c>
-      <c r="D35" s="1">
-        <v>0.87083333333333324</v>
-      </c>
-      <c r="E35" s="1">
-        <f t="shared" si="1"/>
-        <v>2.6388888888888795E-2</v>
-      </c>
-      <c r="F35" s="2">
-        <v>44979</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="3">
-        <v>17</v>
-      </c>
-      <c r="C36" s="1">
-        <v>0.87152777777777779</v>
-      </c>
-      <c r="D36" s="1">
-        <v>0.89097222222222217</v>
-      </c>
-      <c r="E36" s="1">
-        <f t="shared" si="1"/>
-        <v>1.9444444444444375E-2</v>
-      </c>
-      <c r="F36" s="2">
-        <v>44979</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="3">
-        <v>21</v>
-      </c>
-      <c r="C37" s="1">
-        <v>0.90069444444444446</v>
-      </c>
-      <c r="D37" s="1">
-        <v>0.9375</v>
-      </c>
-      <c r="E37" s="1">
-        <f t="shared" si="1"/>
-        <v>3.6805555555555536E-2</v>
-      </c>
-      <c r="F37" s="2">
-        <v>44979</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="3">
-        <v>20</v>
-      </c>
-      <c r="C38" s="1">
-        <v>0.95486111111111116</v>
-      </c>
-      <c r="D38" s="1">
-        <v>0.98333333333333339</v>
-      </c>
-      <c r="E38" s="1">
-        <f t="shared" si="1"/>
-        <v>2.8472222222222232E-2</v>
-      </c>
-      <c r="F38" s="2">
-        <v>44979</v>
-      </c>
-      <c r="G38" s="1">
-        <f>SUM(E28:E38)</f>
-        <v>0.21388888888888857</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" s="3">
-        <v>20</v>
-      </c>
-      <c r="C39" s="1">
-        <v>0.45277777777777778</v>
-      </c>
-      <c r="D39" s="1">
-        <v>0.4826388888888889</v>
-      </c>
-      <c r="E39" s="1">
-        <f t="shared" si="1"/>
-        <v>2.9861111111111116E-2</v>
-      </c>
-      <c r="F39" s="2">
-        <v>44980</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" s="3">
-        <v>15</v>
-      </c>
-      <c r="C40" s="1">
-        <v>0.49027777777777781</v>
-      </c>
-      <c r="D40" s="1">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="E40" s="1">
-        <f t="shared" si="1"/>
-        <v>2.3611111111111138E-2</v>
-      </c>
-      <c r="F40" s="2">
-        <v>44980</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="3">
-        <v>16</v>
-      </c>
-      <c r="C41" s="1">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="D41" s="1">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="E41" s="1">
-        <f t="shared" si="1"/>
-        <v>2.0833333333333259E-2</v>
-      </c>
-      <c r="F41" s="2">
-        <v>44980</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="3">
-        <v>17</v>
-      </c>
-      <c r="C42" s="1">
-        <v>0.54791666666666672</v>
-      </c>
-      <c r="D42" s="1">
-        <v>0.56319444444444444</v>
-      </c>
-      <c r="E42" s="1">
-        <f t="shared" si="1"/>
-        <v>1.5277777777777724E-2</v>
-      </c>
-      <c r="F42" s="2">
-        <v>44980</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" s="3">
-        <v>17</v>
-      </c>
-      <c r="C43" s="1">
-        <v>0.63611111111111118</v>
-      </c>
-      <c r="D43" s="1">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="E43" s="1">
-        <f t="shared" si="1"/>
-        <v>3.0555555555555447E-2</v>
-      </c>
-      <c r="F43" s="2">
-        <v>44980</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="3">
-        <v>14</v>
-      </c>
-      <c r="C44" s="1">
-        <v>0.67083333333333339</v>
-      </c>
-      <c r="D44" s="1">
-        <v>0.68472222222222223</v>
-      </c>
-      <c r="E44" s="1">
-        <f t="shared" si="1"/>
-        <v>1.388888888888884E-2</v>
-      </c>
-      <c r="F44" s="2">
-        <v>44980</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="3">
-        <v>17</v>
-      </c>
-      <c r="C45" s="1">
-        <v>0.69444444444444453</v>
-      </c>
-      <c r="D45" s="1">
-        <v>0.69930555555555562</v>
-      </c>
-      <c r="E45" s="1">
-        <f t="shared" si="1"/>
-        <v>4.8611111111110938E-3</v>
-      </c>
-      <c r="F45" s="2">
-        <v>44980</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F46" s="2">
-        <v>44980</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B47" s="3">
-        <f>SUM(B2:B45)</f>
-        <v>316</v>
-      </c>
-      <c r="F47" s="2">
-        <v>44980</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F48" s="2">
-        <v>44980</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B49" s="3">
-        <f>B47/60</f>
-        <v>5.2666666666666666</v>
-      </c>
-      <c r="F49" s="2">
-        <v>44980</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F50" s="2">
-        <v>44980</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="G51" s="1">
-        <f>SUM(E39:E45)</f>
-        <v>0.13888888888888862</v>
-      </c>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E45" s="1"/>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="G51" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1277,7 +982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB441E67-A5E4-4DE3-B82F-CDFFD92B24D6}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
aula sobre fundos com imagens
</commit_message>
<xml_diff>
--- a/agenda controle.xlsx
+++ b/agenda controle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguia\Documents\GitHub\ProjetosEstudos\module1--html5---css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F7774A-D6DE-4A52-A07E-66E2947801EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF72342-70A7-4384-A487-C76A1E3312AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23235" yWindow="-12360" windowWidth="18690" windowHeight="9990" xr2:uid="{FD96FF53-C3B6-47FE-BDDB-316B30E4002C}"/>
+    <workbookView xWindow="23235" yWindow="-12360" windowWidth="15705" windowHeight="11280" xr2:uid="{FD96FF53-C3B6-47FE-BDDB-316B30E4002C}"/>
   </bookViews>
   <sheets>
     <sheet name="module3" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>Total</t>
   </si>
@@ -211,6 +211,21 @@
   </si>
   <si>
     <t>Capítulo 19 Aula 01- Download das imagens do capítulo</t>
+  </si>
+  <si>
+    <t>Capítulo 19 Aula 02 – Colocando uma imagem de fundo no seu site</t>
+  </si>
+  <si>
+    <t>Capítulo 19 Aula 03 – Imagens que se repetem no fundo do site</t>
+  </si>
+  <si>
+    <t>Capítulo 19 Aula 04 – Configurando a posição da imagem no fundo do site</t>
+  </si>
+  <si>
+    <t>Capítulo 19 Aula 05 – Mudando o tamanho da imagem de fundo do site</t>
+  </si>
+  <si>
+    <t>Capítulo 19 Aula 06 – background-attachment e shorthand</t>
   </si>
 </sst>
 </file>
@@ -574,7 +589,7 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -635,7 +650,7 @@
         <v>0.76250000000000007</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E17" si="0">D3-C3</f>
+        <f t="shared" ref="E3:E18" si="0">D3-C3</f>
         <v>9.7222222222222987E-3</v>
       </c>
       <c r="F3" s="2">
@@ -842,90 +857,173 @@
         <v>0.94027777777777777</v>
       </c>
       <c r="D13" s="1">
-        <v>0.94027777777777777</v>
+        <v>0.9458333333333333</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
+        <v>5.5555555555555358E-3</v>
+      </c>
+      <c r="F13" s="2">
+        <v>44980</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="3">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.9458333333333333</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.95694444444444438</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1111111111111072E-2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>44980</v>
+      </c>
+      <c r="G14" s="1">
+        <f>SUM(E2:E14)+module2!G51</f>
+        <v>0.27083333333333304</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="3">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1">
         <v>0</v>
       </c>
-      <c r="F13" s="2">
-        <v>44980</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="E14" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="2">
-        <v>44980</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D15" s="1">
+        <v>6.2499999999999995E-3</v>
+      </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.2499999999999995E-3</v>
       </c>
       <c r="F15" s="2">
-        <v>44980</v>
+        <v>44981</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="4"/>
-      <c r="E16" s="1"/>
+      <c r="A16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="3">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3.5416666666666666E-2</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>44981</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="E18" s="1"/>
-      <c r="G18" s="1">
-        <f>SUM(E2:E18)+module2!G51</f>
-        <v>0.25416666666666643</v>
-      </c>
-    </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="3">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.55833333333333335</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.57500000000000007</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666718E-2</v>
+      </c>
+      <c r="F17" s="2">
+        <v>44981</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="3">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.5756944444444444</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.58750000000000002</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1805555555555625E-2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>44981</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F19" s="2">
+        <v>44981</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F20" s="2">
+        <v>44981</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="5:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
media query em diferentes orientacoes
</commit_message>
<xml_diff>
--- a/agenda controle.xlsx
+++ b/agenda controle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguia\Documents\GitHub\ProjetosEstudos\module1--html5---css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5EC1B3-59CE-4DB2-B7D9-09A035D813B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC079FA-89E9-4ADB-9CA0-B9A387F116A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16470" yWindow="-15375" windowWidth="22155" windowHeight="13590" xr2:uid="{FD96FF53-C3B6-47FE-BDDB-316B30E4002C}"/>
+    <workbookView xWindow="14070" yWindow="-15720" windowWidth="14700" windowHeight="10080" xr2:uid="{FD96FF53-C3B6-47FE-BDDB-316B30E4002C}"/>
   </bookViews>
   <sheets>
     <sheet name="module4" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="118">
   <si>
     <t>Total</t>
   </si>
@@ -389,6 +389,9 @@
   </si>
   <si>
     <t>Capítulo 25 Aula 03 – Múltiplas Media Features com CSS</t>
+  </si>
+  <si>
+    <t>Capítulo 25 Aula 04 – Seguindo a orientação do dispositivo</t>
   </si>
 </sst>
 </file>
@@ -749,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E5DD25-88AC-4F4F-853C-F3BBF1000474}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -813,7 +816,7 @@
         <v>0.70000000000000007</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E30" si="0">D3-C3</f>
+        <f t="shared" ref="E3:E31" si="0">D3-C3</f>
         <v>9.0277777777778567E-3</v>
       </c>
       <c r="F3" s="2">
@@ -1395,6 +1398,24 @@
       <c r="E30" s="1">
         <f t="shared" si="0"/>
         <v>1.041666666666663E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" s="3">
+        <v>14</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.91875000000000007</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1805555555555403E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
menu telas grandes e pequenas
</commit_message>
<xml_diff>
--- a/agenda controle.xlsx
+++ b/agenda controle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguia\Documents\GitHub\ProjetosEstudos\module1--html5---css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C546C4-AC73-4A89-9E0F-837BAE32E9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAACB37B-130D-4ECA-A8F8-6CDFE75301D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="672" yWindow="672" windowWidth="17886" windowHeight="12300" xr2:uid="{FD96FF53-C3B6-47FE-BDDB-316B30E4002C}"/>
+    <workbookView xWindow="672" yWindow="672" windowWidth="14700" windowHeight="10080" xr2:uid="{FD96FF53-C3B6-47FE-BDDB-316B30E4002C}"/>
   </bookViews>
   <sheets>
     <sheet name="module4" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="126">
   <si>
     <t>Total</t>
   </si>
@@ -413,6 +413,9 @@
   </si>
   <si>
     <t>Capítulo 25 Aula 11 – Criando um menu hambúrguer</t>
+  </si>
+  <si>
+    <t>Capítulo 25 Aula 12 – Media Queries para outros dispositivos</t>
   </si>
 </sst>
 </file>
@@ -773,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E5DD25-88AC-4F4F-853C-F3BBF1000474}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -837,7 +840,7 @@
         <v>0.70000000000000007</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E38" si="0">D3-C3</f>
+        <f t="shared" ref="E3:E39" si="0">D3-C3</f>
         <v>9.0277777777778567E-3</v>
       </c>
       <c r="F3" s="2">
@@ -1593,6 +1596,47 @@
         <v>2.083333333333337E-2</v>
       </c>
       <c r="F38" s="2">
+        <v>44989</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>125</v>
+      </c>
+      <c r="B39" s="3">
+        <v>15</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.65486111111111112</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2500000000000067E-2</v>
+      </c>
+      <c r="F39" s="2">
+        <v>44989</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F40" s="2">
+        <v>44989</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F41" s="2">
+        <v>44989</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F42" s="2">
+        <v>44989</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="F43" s="2">
         <v>44989</v>
       </c>
     </row>

</xml_diff>